<commit_message>
add: add button event
</commit_message>
<xml_diff>
--- a/文档/问题记录及解决.xlsx
+++ b/文档/问题记录及解决.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HowtoGetaJob\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A6BED37-9CB1-4C5C-86F3-894B2A94F465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109F6229-02DA-4A36-85FD-182B6D3AE1CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,40 +25,63 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="15">
   <si>
     <t>时间</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>是否已解决</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>解决方式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>补充</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是</t>
+  </si>
+  <si>
+    <t>unity根目录下Library内二进制文件大于100M，无法存入git仓库</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在vs中有一个Git更改，通过设置.gitignore忽略文件，在vs里commit，在sourcetree里push就ok</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>文件必须放在unity项目根目录下（或许在路径前加上前缀也行？）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>否</t>
+  </si>
+  <si>
+    <t>问题描述</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>问题类型</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>是否已解决</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>解决方式</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>补充</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>是</t>
-  </si>
-  <si>
-    <t>unity根目录下Library内二进制文件大于100M，无法存入git仓库</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>在vs中有一个Git更改，通过设置.gitignore忽略文件，在vs里commit，在sourcetree里push就ok</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>文件必须放在unity项目根目录下（或许在路径前加上前缀也行？）</t>
+    <t>技术问题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>体验问题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重录视频，重做UI。考虑以后做一测一，避免连带资源重做</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开始视频3840x2160，游戏1624X750，未能提前预知风险，视频效果糟糕（卡顿闪烁），且视频拍摄手法生疏，考虑重做。登陆界面UI依赖视频最后一帧，所以UI需重做</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -108,7 +131,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -127,6 +150,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -408,91 +434,260 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="47" style="3" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="41.6640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="31.6640625" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="2" width="21.5546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="47" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="41.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="31.6640625" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
-    </row>
-    <row r="2" spans="1:10" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K1" s="2"/>
+    </row>
+    <row r="2" spans="1:11" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>44961</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="61.2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:10" ht="61.2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:10" ht="61.2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:10" ht="61.2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:10" ht="61.2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:10" ht="61.2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:10" ht="61.2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:10" ht="61.2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:10" ht="61.2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:10" ht="61.2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:10" ht="61.2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:10" ht="61.2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:10" ht="61.2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:10" ht="61.2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="61.2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="61.2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="61.2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="61.2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="61.2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="61.2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="61.2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="61.2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="61.2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" ht="61.2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" ht="61.2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" ht="61.2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" ht="61.2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" ht="61.2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" ht="61.2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" ht="61.2" customHeight="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="3" spans="1:11" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>44962</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:11" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:11" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:11" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:11" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:11" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:11" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="7"/>
+      <c r="D9" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="7"/>
+      <c r="D10" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="7"/>
+      <c r="D11" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="7"/>
+      <c r="D12" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="7"/>
+      <c r="D13" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="7"/>
+      <c r="D14" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="7"/>
+      <c r="D15" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="7"/>
+      <c r="D16" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="7"/>
+      <c r="D17" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="7"/>
+      <c r="D18" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="7"/>
+      <c r="D19" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="7"/>
+      <c r="D20" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="7"/>
+      <c r="D21" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="7"/>
+      <c r="D22" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="7"/>
+      <c r="D23" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="7"/>
+      <c r="D24" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="3:4" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="7"/>
+      <c r="D25" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="3:4" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D26" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="3:4" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D27" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="3:4" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D28" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="3:4" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D29" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="3:4" ht="61.2" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="3:4" ht="61.2" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="3:4" ht="61.2" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="61.2" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="61.2" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="61.2" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -500,7 +695,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{8BE2B081-C4C7-4627-914F-314CEEE85100}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D29" xr:uid="{8BE2B081-C4C7-4627-914F-314CEEE85100}">
       <formula1>"是,否"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
add: add new player art, new player prefab, update doc
</commit_message>
<xml_diff>
--- a/文档/问题记录及解决.xlsx
+++ b/文档/问题记录及解决.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HowtoGetaJob\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BE1741-4795-47A2-9FCC-FB8F90D401FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{998EED7C-AA03-4557-BED9-4D9833BC40E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="22">
   <si>
     <t>时间</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -54,10 +54,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>文件必须放在unity项目根目录下（或许在路径前加上前缀也行？）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>否</t>
   </si>
   <si>
@@ -93,11 +89,28 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>使用Avpro插件播放视频</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>有水印，正在解决</t>
+    <t>使用Avpro插件播放视频，但有水印，正在解决</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用回VideoPlayer后安卓机上又出现视频了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>技术问题
+渲染顺序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用的sprite skin，人物朝左，理应左手在上，右手遮挡部分不可见，然而无论怎么调顺序双手都在身体下面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在sprite editor面板修改骨骼的depth属性，即可改变骨骼间的层级</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>忽略文件路径为，以所在目录为根目录的，相对路径</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -453,7 +466,7 @@
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -471,10 +484,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -493,10 +506,10 @@
     </row>
     <row r="2" spans="1:11" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
-        <v>44961</v>
+        <v>44981</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>5</v>
@@ -508,55 +521,63 @@
         <v>6</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
-        <v>44962</v>
+        <v>44982</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:11" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <v>44962</v>
+        <v>44982</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="6" t="s">
+    </row>
+    <row r="5" spans="1:11" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>44984</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="5"/>
+      <c r="C5" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="D5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="6"/>
+        <v>4</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:11" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -564,7 +585,7 @@
       <c r="B6" s="6"/>
       <c r="C6" s="5"/>
       <c r="D6" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -574,7 +595,7 @@
       <c r="B7" s="6"/>
       <c r="C7" s="5"/>
       <c r="D7" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -584,7 +605,7 @@
       <c r="B8" s="6"/>
       <c r="C8" s="5"/>
       <c r="D8" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -592,123 +613,123 @@
     <row r="9" spans="1:11" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="7"/>
       <c r="D9" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="7"/>
       <c r="D10" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="7"/>
       <c r="D11" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="7"/>
       <c r="D12" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="7"/>
       <c r="D13" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="7"/>
       <c r="D14" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="7"/>
       <c r="D15" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="7"/>
       <c r="D16" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="3:4" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="7"/>
       <c r="D17" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="3:4" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="7"/>
       <c r="D18" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="3:4" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="7"/>
       <c r="D19" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="3:4" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="7"/>
       <c r="D20" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="3:4" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="7"/>
       <c r="D21" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="3:4" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="7"/>
       <c r="D22" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="3:4" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="7"/>
       <c r="D23" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="3:4" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="7"/>
       <c r="D24" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="3:4" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="7"/>
       <c r="D25" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="3:4" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D26" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="3:4" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D27" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="3:4" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D28" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="3:4" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D29" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="3:4" ht="61.2" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>